<commit_message>
Testes para o req. : Associação de clientes a exercícios concluidos
</commit_message>
<xml_diff>
--- a/testes/AS_associar_exercicio_cliente_equipamento.xlsx
+++ b/testes/AS_associar_exercicio_cliente_equipamento.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="86">
   <si>
     <t>Sistema:</t>
   </si>
@@ -209,9 +209,6 @@
     <t>O sistema exibe uma nova tela com as associações existentes.</t>
   </si>
   <si>
-    <t>CT008, o Usuário Adm seleciona o registro a ser atualizado.</t>
-  </si>
-  <si>
     <t>O sistem exibe a tela de associação em modo de atualização, com os dados do registro selecionado devidamente preenchidos.</t>
   </si>
   <si>
@@ -278,9 +275,6 @@
     <t>RESULTADO DOS TESTES</t>
   </si>
   <si>
-    <t>Sucesso</t>
-  </si>
-  <si>
     <t>Digitar o nome do exercício no respectivo campo</t>
   </si>
   <si>
@@ -290,7 +284,76 @@
     <t>Digitar o nome do equipamento no respectivo campo</t>
   </si>
   <si>
-    <t>Erro</t>
+    <t>CT008, o Usuário Adm clica no registro a ser atualizado.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Resultado dos testes  -  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Verde : Sucesso</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> /  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Vermelho : Erro</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="3" tint="0.39997558519241921"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Azul : Ainda não testado</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="3" tint="0.39997558519241921"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -300,7 +363,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\C\T000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -366,8 +429,54 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="3" tint="0.39997558519241921"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="3" tint="0.39997558519241921"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="3" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -431,12 +540,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1100,7 +1203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1270,35 +1373,11 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="11" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="8" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="8" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1307,37 +1386,6 @@
     <xf numFmtId="164" fontId="8" fillId="8" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="8" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="8" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="8" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1347,7 +1395,56 @@
     <xf numFmtId="49" fontId="9" fillId="8" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="9" fillId="8" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1357,63 +1454,78 @@
     <xf numFmtId="49" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="8" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2261,10 +2373,10 @@
   <dimension ref="A1:HV118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="F31" sqref="F31:F33"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2283,12 +2395,12 @@
       <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="110" t="s">
+      <c r="B1" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="108" t="s">
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="85" t="s">
         <v>21</v>
       </c>
       <c r="J1" s="1"/>
@@ -2513,14 +2625,16 @@
       <c r="HU1" s="1"/>
       <c r="HV1" s="1"/>
     </row>
-    <row r="2" spans="1:230" s="7" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:230" s="7" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="113"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="108"/>
+      <c r="B2" s="128" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="89"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="85"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -2744,13 +2858,13 @@
       <c r="HV2" s="1"/>
     </row>
     <row r="3" spans="1:230" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="106" t="s">
+      <c r="A3" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="115"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="117"/>
-      <c r="E3" s="108"/>
+      <c r="B3" s="91"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="85"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -2974,11 +3088,11 @@
       <c r="HV3" s="1"/>
     </row>
     <row r="4" spans="1:230" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="107"/>
-      <c r="B4" s="118"/>
-      <c r="C4" s="119"/>
-      <c r="D4" s="120"/>
-      <c r="E4" s="109"/>
+      <c r="A4" s="84"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="86"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -3202,13 +3316,13 @@
       <c r="HV4" s="1"/>
     </row>
     <row r="5" spans="1:230" s="4" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="121" t="s">
+      <c r="A5" s="97" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="122"/>
-      <c r="C5" s="122"/>
-      <c r="D5" s="122"/>
-      <c r="E5" s="122"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -3448,7 +3562,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="68" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -3676,10 +3790,10 @@
       <c r="A7" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="93" t="s">
+      <c r="B7" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="93" t="s">
+      <c r="C7" s="75" t="s">
         <v>35</v>
       </c>
       <c r="D7" s="46" t="s">
@@ -3688,9 +3802,7 @@
       <c r="E7" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="75" t="s">
-        <v>82</v>
-      </c>
+      <c r="F7" s="126"/>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
@@ -3915,11 +4027,11 @@
     </row>
     <row r="8" spans="1:230" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="72"/>
-      <c r="B8" s="92"/>
-      <c r="C8" s="92"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
       <c r="D8" s="46"/>
       <c r="E8" s="48"/>
-      <c r="F8" s="76"/>
+      <c r="F8" s="117"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
@@ -4144,11 +4256,11 @@
     </row>
     <row r="9" spans="1:230" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="72"/>
-      <c r="B9" s="92"/>
-      <c r="C9" s="92"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
       <c r="D9" s="46"/>
       <c r="E9" s="48"/>
-      <c r="F9" s="76"/>
+      <c r="F9" s="117"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
@@ -4604,10 +4716,10 @@
       <c r="A11" s="71">
         <v>2</v>
       </c>
-      <c r="B11" s="93" t="s">
+      <c r="B11" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="93" t="s">
+      <c r="C11" s="75" t="s">
         <v>51</v>
       </c>
       <c r="D11" s="46" t="s">
@@ -4616,9 +4728,7 @@
       <c r="E11" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="77" t="s">
-        <v>82</v>
-      </c>
+      <c r="F11" s="127"/>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
@@ -4843,13 +4953,13 @@
     </row>
     <row r="12" spans="1:230" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="72"/>
-      <c r="B12" s="92"/>
-      <c r="C12" s="92"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
       <c r="D12" s="46" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E12" s="47"/>
-      <c r="F12" s="78"/>
+      <c r="F12" s="118"/>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
@@ -5074,13 +5184,13 @@
     </row>
     <row r="13" spans="1:230" s="8" customFormat="1" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="72"/>
-      <c r="B13" s="92"/>
-      <c r="C13" s="92"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="76"/>
       <c r="D13" s="46" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="47"/>
-      <c r="F13" s="78"/>
+      <c r="F13" s="118"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
@@ -5533,13 +5643,13 @@
       <c r="HV14"/>
     </row>
     <row r="15" spans="1:230" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="123" t="s">
+      <c r="A15" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="99" t="s">
+      <c r="B15" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="99" t="s">
+      <c r="C15" s="80" t="s">
         <v>52</v>
       </c>
       <c r="D15" s="46" t="s">
@@ -5548,9 +5658,7 @@
       <c r="E15" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="75" t="s">
-        <v>82</v>
-      </c>
+      <c r="F15" s="126"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
@@ -5774,14 +5882,14 @@
       <c r="HV15" s="12"/>
     </row>
     <row r="16" spans="1:230" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="86"/>
-      <c r="B16" s="100"/>
-      <c r="C16" s="100"/>
+      <c r="A16" s="78"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="81"/>
       <c r="D16" s="46" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E16" s="48"/>
-      <c r="F16" s="76"/>
+      <c r="F16" s="117"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
@@ -6005,12 +6113,12 @@
       <c r="HV16" s="12"/>
     </row>
     <row r="17" spans="1:230" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="87"/>
-      <c r="B17" s="101"/>
-      <c r="C17" s="101"/>
+      <c r="A17" s="79"/>
+      <c r="B17" s="82"/>
+      <c r="C17" s="82"/>
       <c r="D17" s="46"/>
       <c r="E17" s="48"/>
-      <c r="F17" s="76"/>
+      <c r="F17" s="117"/>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
@@ -6466,10 +6574,10 @@
       <c r="A19" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="93" t="s">
+      <c r="B19" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="93" t="s">
+      <c r="C19" s="75" t="s">
         <v>53</v>
       </c>
       <c r="D19" s="46" t="s">
@@ -6478,9 +6586,7 @@
       <c r="E19" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="75" t="s">
-        <v>82</v>
-      </c>
+      <c r="F19" s="116"/>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
@@ -6705,13 +6811,13 @@
     </row>
     <row r="20" spans="1:230" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="72"/>
-      <c r="B20" s="92"/>
-      <c r="C20" s="92"/>
+      <c r="B20" s="76"/>
+      <c r="C20" s="76"/>
       <c r="D20" s="46" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E20" s="48"/>
-      <c r="F20" s="76"/>
+      <c r="F20" s="117"/>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
@@ -6936,11 +7042,11 @@
     </row>
     <row r="21" spans="1:230" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="72"/>
-      <c r="B21" s="92"/>
-      <c r="C21" s="92"/>
+      <c r="B21" s="76"/>
+      <c r="C21" s="76"/>
       <c r="D21" s="46"/>
       <c r="E21" s="48"/>
-      <c r="F21" s="76"/>
+      <c r="F21" s="117"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
@@ -7396,10 +7502,10 @@
       <c r="A23" s="71">
         <v>5</v>
       </c>
-      <c r="B23" s="93" t="s">
+      <c r="B23" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="93" t="s">
+      <c r="C23" s="75" t="s">
         <v>37</v>
       </c>
       <c r="D23" s="46" t="s">
@@ -7408,29 +7514,27 @@
       <c r="E23" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="79" t="s">
-        <v>82</v>
-      </c>
+      <c r="F23" s="119"/>
     </row>
     <row r="24" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="72"/>
-      <c r="B24" s="92"/>
-      <c r="C24" s="92"/>
+      <c r="B24" s="76"/>
+      <c r="C24" s="76"/>
       <c r="D24" s="46" t="s">
         <v>39</v>
       </c>
       <c r="E24" s="48"/>
-      <c r="F24" s="80"/>
+      <c r="F24" s="120"/>
     </row>
     <row r="25" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="72"/>
-      <c r="B25" s="92"/>
-      <c r="C25" s="92"/>
+      <c r="B25" s="76"/>
+      <c r="C25" s="76"/>
       <c r="D25" s="46" t="s">
         <v>40</v>
       </c>
       <c r="E25" s="48"/>
-      <c r="F25" s="80"/>
+      <c r="F25" s="120"/>
     </row>
     <row r="26" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="37"/>
@@ -7444,10 +7548,10 @@
       <c r="A27" s="71">
         <v>6</v>
       </c>
-      <c r="B27" s="93" t="s">
+      <c r="B27" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="93" t="s">
+      <c r="C27" s="75" t="s">
         <v>43</v>
       </c>
       <c r="D27" s="46" t="s">
@@ -7456,29 +7560,27 @@
       <c r="E27" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="79" t="s">
-        <v>82</v>
-      </c>
+      <c r="F27" s="119"/>
     </row>
     <row r="28" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="72"/>
-      <c r="B28" s="92"/>
-      <c r="C28" s="92"/>
+      <c r="B28" s="76"/>
+      <c r="C28" s="76"/>
       <c r="D28" s="46" t="s">
         <v>45</v>
       </c>
       <c r="E28" s="48"/>
-      <c r="F28" s="81"/>
+      <c r="F28" s="121"/>
     </row>
     <row r="29" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="72"/>
-      <c r="B29" s="92"/>
-      <c r="C29" s="92"/>
+      <c r="B29" s="76"/>
+      <c r="C29" s="76"/>
       <c r="D29" s="46" t="s">
         <v>40</v>
       </c>
       <c r="E29" s="48"/>
-      <c r="F29" s="81"/>
+      <c r="F29" s="121"/>
     </row>
     <row r="30" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="37"/>
@@ -7491,10 +7593,10 @@
       <c r="A31" s="71">
         <v>7</v>
       </c>
-      <c r="B31" s="93" t="s">
+      <c r="B31" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="93" t="s">
+      <c r="C31" s="75" t="s">
         <v>47</v>
       </c>
       <c r="D31" s="46" t="s">
@@ -7503,47 +7605,45 @@
       <c r="E31" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="F31" s="124" t="s">
-        <v>86</v>
-      </c>
+      <c r="F31" s="119"/>
     </row>
     <row r="32" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="103"/>
-      <c r="B32" s="92"/>
-      <c r="C32" s="92"/>
+      <c r="A32" s="101"/>
+      <c r="B32" s="76"/>
+      <c r="C32" s="76"/>
       <c r="D32" s="46" t="s">
         <v>45</v>
       </c>
       <c r="E32" s="48"/>
-      <c r="F32" s="125"/>
+      <c r="F32" s="121"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="103"/>
-      <c r="B33" s="92"/>
-      <c r="C33" s="92"/>
+      <c r="A33" s="101"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="76"/>
       <c r="D33" s="46" t="s">
         <v>40</v>
       </c>
       <c r="E33" s="48"/>
-      <c r="F33" s="125"/>
+      <c r="F33" s="121"/>
     </row>
     <row r="34" spans="1:6" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="104" t="s">
+      <c r="A34" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="105"/>
-      <c r="C34" s="105"/>
-      <c r="D34" s="105"/>
-      <c r="E34" s="105"/>
+      <c r="B34" s="103"/>
+      <c r="C34" s="103"/>
+      <c r="D34" s="103"/>
+      <c r="E34" s="103"/>
     </row>
     <row r="35" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="71">
         <v>8</v>
       </c>
-      <c r="B35" s="93" t="s">
+      <c r="B35" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="93" t="s">
+      <c r="C35" s="75" t="s">
         <v>50</v>
       </c>
       <c r="D35" s="46" t="s">
@@ -7552,27 +7652,31 @@
       <c r="E35" s="48" t="s">
         <v>58</v>
       </c>
+      <c r="F35" s="125"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="72"/>
-      <c r="B36" s="92"/>
-      <c r="C36" s="92"/>
+      <c r="B36" s="76"/>
+      <c r="C36" s="76"/>
       <c r="D36" s="46"/>
       <c r="E36" s="48"/>
+      <c r="F36" s="121"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="72"/>
-      <c r="B37" s="92"/>
-      <c r="C37" s="92"/>
+      <c r="B37" s="76"/>
+      <c r="C37" s="76"/>
       <c r="D37" s="46"/>
       <c r="E37" s="48"/>
+      <c r="F37" s="121"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="72"/>
-      <c r="B38" s="92"/>
-      <c r="C38" s="92"/>
+      <c r="B38" s="76"/>
+      <c r="C38" s="76"/>
       <c r="D38" s="46"/>
       <c r="E38" s="48"/>
+      <c r="F38" s="121"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="37"/>
@@ -7585,34 +7689,37 @@
       <c r="A40" s="71">
         <v>9</v>
       </c>
-      <c r="B40" s="93" t="s">
+      <c r="B40" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="102" t="s">
+      <c r="C40" s="99" t="s">
         <v>54</v>
       </c>
       <c r="D40" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="E40" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="E40" s="48" t="s">
-        <v>60</v>
-      </c>
+      <c r="F40" s="125"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="72"/>
-      <c r="B41" s="92"/>
-      <c r="C41" s="100"/>
+      <c r="B41" s="76"/>
+      <c r="C41" s="81"/>
       <c r="D41" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E41" s="48"/>
+      <c r="F41" s="121"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="72"/>
-      <c r="B42" s="92"/>
-      <c r="C42" s="91"/>
+      <c r="B42" s="76"/>
+      <c r="C42" s="100"/>
       <c r="D42" s="46"/>
       <c r="E42" s="48"/>
+      <c r="F42" s="121"/>
     </row>
     <row r="43" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="37"/>
@@ -7625,35 +7732,35 @@
       <c r="A44" s="71">
         <v>10</v>
       </c>
-      <c r="B44" s="99" t="s">
+      <c r="B44" s="80" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="99" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="C44" s="102" t="s">
-        <v>50</v>
-      </c>
-      <c r="D44" s="46" t="s">
+      <c r="E44" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="E44" s="48" t="s">
-        <v>63</v>
-      </c>
-      <c r="F44" s="51"/>
+      <c r="F44" s="120"/>
     </row>
     <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="72"/>
-      <c r="B45" s="100"/>
-      <c r="C45" s="100"/>
+      <c r="B45" s="81"/>
+      <c r="C45" s="81"/>
       <c r="D45" s="46"/>
       <c r="E45" s="48"/>
-      <c r="F45" s="51"/>
+      <c r="F45" s="120"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="72"/>
-      <c r="B46" s="101"/>
-      <c r="C46" s="101"/>
+      <c r="B46" s="82"/>
+      <c r="C46" s="82"/>
       <c r="D46" s="52"/>
       <c r="E46" s="48"/>
-      <c r="F46" s="51"/>
+      <c r="F46" s="120"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="37"/>
@@ -7667,35 +7774,35 @@
       <c r="A48" s="71">
         <v>11</v>
       </c>
-      <c r="B48" s="94" t="s">
+      <c r="B48" s="106" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48" s="106" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="94" t="s">
+      <c r="D48" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="E48" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="D48" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="E48" s="48" t="s">
-        <v>66</v>
-      </c>
-      <c r="F48" s="51"/>
+      <c r="F48" s="120"/>
     </row>
     <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="72"/>
-      <c r="B49" s="95"/>
-      <c r="C49" s="95"/>
+      <c r="B49" s="107"/>
+      <c r="C49" s="107"/>
       <c r="D49" s="46"/>
       <c r="E49" s="48"/>
-      <c r="F49" s="51"/>
+      <c r="F49" s="120"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="72"/>
-      <c r="B50" s="96"/>
-      <c r="C50" s="96"/>
+      <c r="B50" s="108"/>
+      <c r="C50" s="108"/>
       <c r="D50" s="52"/>
       <c r="E50" s="53"/>
-      <c r="F50" s="51"/>
+      <c r="F50" s="120"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="37"/>
@@ -7709,85 +7816,85 @@
       <c r="A52" s="71">
         <v>12</v>
       </c>
-      <c r="B52" s="97" t="s">
+      <c r="B52" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="98" t="s">
-        <v>67</v>
+      <c r="C52" s="105" t="s">
+        <v>66</v>
       </c>
       <c r="D52" s="55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E52" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="F52" s="51"/>
+      <c r="F52" s="123"/>
     </row>
     <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="72"/>
-      <c r="B53" s="97"/>
-      <c r="C53" s="98"/>
+      <c r="B53" s="104"/>
+      <c r="C53" s="105"/>
       <c r="D53" s="57"/>
       <c r="E53" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="F53" s="51"/>
+      <c r="F53" s="123"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="72"/>
-      <c r="B54" s="97"/>
-      <c r="C54" s="98"/>
+      <c r="B54" s="104"/>
+      <c r="C54" s="105"/>
       <c r="D54" s="58"/>
       <c r="E54" s="59"/>
-      <c r="F54" s="51"/>
+      <c r="F54" s="123"/>
     </row>
     <row r="55" spans="1:6" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="83" t="s">
-        <v>68</v>
-      </c>
-      <c r="B55" s="84"/>
-      <c r="C55" s="84"/>
-      <c r="D55" s="84"/>
-      <c r="E55" s="84"/>
+      <c r="A55" s="109" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" s="110"/>
+      <c r="C55" s="110"/>
+      <c r="D55" s="110"/>
+      <c r="E55" s="110"/>
       <c r="F55" s="51"/>
     </row>
     <row r="56" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A56" s="71">
         <v>13</v>
       </c>
-      <c r="B56" s="97" t="s">
+      <c r="B56" s="104" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="C56" s="98" t="s">
+      <c r="D56" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="D56" s="55" t="s">
-        <v>71</v>
-      </c>
       <c r="E56" s="60" t="s">
-        <v>78</v>
-      </c>
-      <c r="F56" s="51"/>
+        <v>77</v>
+      </c>
+      <c r="F56" s="122"/>
     </row>
     <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="72"/>
-      <c r="B57" s="97"/>
-      <c r="C57" s="98"/>
+      <c r="B57" s="104"/>
+      <c r="C57" s="105"/>
       <c r="D57" s="61" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E57" s="62"/>
-      <c r="F57" s="51"/>
+      <c r="F57" s="122"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="72"/>
-      <c r="B58" s="97"/>
-      <c r="C58" s="98"/>
+      <c r="B58" s="104"/>
+      <c r="C58" s="105"/>
       <c r="D58" s="63" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E58" s="64"/>
-      <c r="F58" s="51"/>
+      <c r="F58" s="122"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="37"/>
@@ -7801,39 +7908,39 @@
       <c r="A60" s="71">
         <v>14</v>
       </c>
-      <c r="B60" s="97" t="s">
+      <c r="B60" s="104" t="s">
+        <v>72</v>
+      </c>
+      <c r="C60" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="C60" s="98" t="s">
-        <v>74</v>
-      </c>
       <c r="D60" s="66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E60" s="66" t="s">
-        <v>78</v>
-      </c>
-      <c r="F60" s="51"/>
+        <v>77</v>
+      </c>
+      <c r="F60" s="124"/>
     </row>
     <row r="61" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="72"/>
-      <c r="B61" s="97"/>
-      <c r="C61" s="97"/>
+      <c r="B61" s="104"/>
+      <c r="C61" s="104"/>
       <c r="D61" s="67" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E61" s="67"/>
-      <c r="F61" s="51"/>
+      <c r="F61" s="124"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="72"/>
-      <c r="B62" s="97"/>
-      <c r="C62" s="97"/>
+      <c r="B62" s="104"/>
+      <c r="C62" s="104"/>
       <c r="D62" s="67" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E62" s="67"/>
-      <c r="F62" s="51"/>
+      <c r="F62" s="124"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="37"/>
@@ -7847,39 +7954,39 @@
       <c r="A64" s="71">
         <v>15</v>
       </c>
-      <c r="B64" s="91" t="s">
+      <c r="B64" s="100" t="s">
+        <v>74</v>
+      </c>
+      <c r="C64" s="100" t="s">
         <v>75</v>
       </c>
-      <c r="C64" s="91" t="s">
-        <v>76</v>
-      </c>
       <c r="D64" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E64" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="F64" s="51"/>
+        <v>77</v>
+      </c>
+      <c r="F64" s="120"/>
     </row>
     <row r="65" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="72"/>
-      <c r="B65" s="92"/>
-      <c r="C65" s="92"/>
+      <c r="B65" s="76"/>
+      <c r="C65" s="76"/>
       <c r="D65" s="46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E65" s="48"/>
-      <c r="F65" s="51"/>
+      <c r="F65" s="120"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="72"/>
-      <c r="B66" s="92"/>
-      <c r="C66" s="92"/>
+      <c r="B66" s="76"/>
+      <c r="C66" s="76"/>
       <c r="D66" s="46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E66" s="48"/>
-      <c r="F66" s="51"/>
+      <c r="F66" s="120"/>
     </row>
     <row r="67" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="37"/>
@@ -7893,8 +8000,8 @@
       <c r="A68" s="71">
         <v>16</v>
       </c>
-      <c r="B68" s="93"/>
-      <c r="C68" s="93" t="s">
+      <c r="B68" s="75"/>
+      <c r="C68" s="75" t="s">
         <v>17</v>
       </c>
       <c r="D68" s="46"/>
@@ -7903,16 +8010,16 @@
     </row>
     <row r="69" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="72"/>
-      <c r="B69" s="92"/>
-      <c r="C69" s="92"/>
+      <c r="B69" s="76"/>
+      <c r="C69" s="76"/>
       <c r="D69" s="46"/>
       <c r="E69" s="48"/>
       <c r="F69" s="51"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="72"/>
-      <c r="B70" s="92"/>
-      <c r="C70" s="92"/>
+      <c r="B70" s="76"/>
+      <c r="C70" s="76"/>
       <c r="D70" s="46"/>
       <c r="E70" s="48"/>
       <c r="F70" s="51"/>
@@ -7937,15 +8044,15 @@
     </row>
     <row r="73" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="72"/>
-      <c r="B73" s="82"/>
-      <c r="C73" s="82"/>
+      <c r="B73" s="115"/>
+      <c r="C73" s="115"/>
       <c r="D73" s="40"/>
       <c r="E73" s="41"/>
     </row>
     <row r="74" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="72"/>
-      <c r="B74" s="82"/>
-      <c r="C74" s="82"/>
+      <c r="B74" s="115"/>
+      <c r="C74" s="115"/>
       <c r="D74" s="42" t="s">
         <v>16</v>
       </c>
@@ -7971,15 +8078,15 @@
     </row>
     <row r="77" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="72"/>
-      <c r="B77" s="82"/>
-      <c r="C77" s="82"/>
+      <c r="B77" s="115"/>
+      <c r="C77" s="115"/>
       <c r="D77" s="40"/>
       <c r="E77" s="41"/>
     </row>
     <row r="78" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="72"/>
-      <c r="B78" s="82"/>
-      <c r="C78" s="82"/>
+      <c r="B78" s="115"/>
+      <c r="C78" s="115"/>
       <c r="D78" s="42" t="s">
         <v>16</v>
       </c>
@@ -8247,43 +8354,104 @@
       <c r="E115" s="44"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A116" s="85"/>
-      <c r="B116" s="88"/>
-      <c r="C116" s="88"/>
+      <c r="A116" s="111"/>
+      <c r="B116" s="112"/>
+      <c r="C116" s="112"/>
       <c r="D116" s="40"/>
       <c r="E116" s="41"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A117" s="86"/>
-      <c r="B117" s="89"/>
-      <c r="C117" s="89"/>
+      <c r="A117" s="78"/>
+      <c r="B117" s="113"/>
+      <c r="C117" s="113"/>
       <c r="D117" s="40"/>
       <c r="E117" s="41"/>
     </row>
     <row r="118" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="87"/>
-      <c r="B118" s="90"/>
-      <c r="C118" s="90"/>
+      <c r="A118" s="79"/>
+      <c r="B118" s="114"/>
+      <c r="C118" s="114"/>
       <c r="D118" s="40"/>
       <c r="E118" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="99">
-    <mergeCell ref="A112:A114"/>
-    <mergeCell ref="B112:B114"/>
-    <mergeCell ref="C112:C114"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="B104:B106"/>
-    <mergeCell ref="C104:C106"/>
-    <mergeCell ref="A108:A110"/>
-    <mergeCell ref="B108:B110"/>
-    <mergeCell ref="C108:C110"/>
-    <mergeCell ref="A92:A94"/>
-    <mergeCell ref="B92:B94"/>
-    <mergeCell ref="C92:C94"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="B96:B98"/>
-    <mergeCell ref="C96:C98"/>
+  <mergeCells count="107">
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="F60:F62"/>
+    <mergeCell ref="F64:F66"/>
+    <mergeCell ref="F35:F38"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="F48:F50"/>
+    <mergeCell ref="F52:F54"/>
+    <mergeCell ref="A88:A90"/>
+    <mergeCell ref="B88:B90"/>
+    <mergeCell ref="C88:C90"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="F31:F33"/>
+    <mergeCell ref="A76:A78"/>
+    <mergeCell ref="B76:B78"/>
+    <mergeCell ref="C76:C78"/>
+    <mergeCell ref="A80:A82"/>
+    <mergeCell ref="B80:B82"/>
+    <mergeCell ref="C80:C82"/>
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="A116:A118"/>
+    <mergeCell ref="B116:B118"/>
+    <mergeCell ref="C116:C118"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="C72:C74"/>
+    <mergeCell ref="A64:A66"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="C64:C66"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="C68:C70"/>
+    <mergeCell ref="A84:A86"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="C84:C86"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="C52:C54"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="C56:C58"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="C60:C62"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="E1:E4"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D4"/>
+    <mergeCell ref="A5:E5"/>
     <mergeCell ref="A100:A102"/>
     <mergeCell ref="B100:B102"/>
     <mergeCell ref="C100:C102"/>
@@ -8300,74 +8468,21 @@
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="E1:E4"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="C60:C62"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="C52:C54"/>
-    <mergeCell ref="A55:E55"/>
-    <mergeCell ref="A116:A118"/>
-    <mergeCell ref="B116:B118"/>
-    <mergeCell ref="C116:C118"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="C72:C74"/>
-    <mergeCell ref="A64:A66"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="C64:C66"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="A84:A86"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="C84:C86"/>
-    <mergeCell ref="A88:A90"/>
-    <mergeCell ref="B88:B90"/>
-    <mergeCell ref="C88:C90"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="A76:A78"/>
-    <mergeCell ref="B76:B78"/>
-    <mergeCell ref="C76:C78"/>
-    <mergeCell ref="A80:A82"/>
-    <mergeCell ref="B80:B82"/>
-    <mergeCell ref="C80:C82"/>
+    <mergeCell ref="A92:A94"/>
+    <mergeCell ref="B92:B94"/>
+    <mergeCell ref="C92:C94"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="B96:B98"/>
+    <mergeCell ref="C96:C98"/>
+    <mergeCell ref="A112:A114"/>
+    <mergeCell ref="B112:B114"/>
+    <mergeCell ref="C112:C114"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="B104:B106"/>
+    <mergeCell ref="C104:C106"/>
+    <mergeCell ref="A108:A110"/>
+    <mergeCell ref="B108:B110"/>
+    <mergeCell ref="C108:C110"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.39370078740157483" bottom="0.39370078740157483" header="0.27559055118110237" footer="0.39370078740157483"/>

</xml_diff>

<commit_message>
concluindo casos de testes para associação e exercicio
</commit_message>
<xml_diff>
--- a/testes/AS_associar_exercicio_cliente_equipamento.xlsx
+++ b/testes/AS_associar_exercicio_cliente_equipamento.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="88">
   <si>
     <t>Sistema:</t>
   </si>
@@ -354,6 +354,12 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t>Os campos do formulário são limpos para uma nova inclusão</t>
+  </si>
+  <si>
+    <t>Campos limpos para uma nova inclusão.</t>
   </si>
 </sst>
 </file>
@@ -1365,6 +1371,24 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="8" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1373,18 +1397,70 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="11" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="8" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="8" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="8" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="8" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="8" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1395,56 +1471,7 @@
     <xf numFmtId="49" fontId="9" fillId="8" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="8" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="8" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1454,78 +1481,57 @@
     <xf numFmtId="49" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="8" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2373,10 +2379,10 @@
   <dimension ref="A1:HV118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2:D2"/>
+      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2395,12 +2401,12 @@
       <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="115" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="85" t="s">
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="113" t="s">
         <v>21</v>
       </c>
       <c r="J1" s="1"/>
@@ -2629,12 +2635,12 @@
       <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="117" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="85"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="113"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -2858,13 +2864,13 @@
       <c r="HV2" s="1"/>
     </row>
     <row r="3" spans="1:230" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="91"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="85"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="121"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="113"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -3088,11 +3094,11 @@
       <c r="HV3" s="1"/>
     </row>
     <row r="4" spans="1:230" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="84"/>
-      <c r="B4" s="94"/>
-      <c r="C4" s="95"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="86"/>
+      <c r="A4" s="112"/>
+      <c r="B4" s="123"/>
+      <c r="C4" s="124"/>
+      <c r="D4" s="125"/>
+      <c r="E4" s="114"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -3316,13 +3322,13 @@
       <c r="HV4" s="1"/>
     </row>
     <row r="5" spans="1:230" s="4" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="97" t="s">
+      <c r="A5" s="126" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="98"/>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="98"/>
+      <c r="B5" s="127"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="127"/>
+      <c r="E5" s="127"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -3787,13 +3793,13 @@
       <c r="HV6" s="1"/>
     </row>
     <row r="7" spans="1:230" s="8" customFormat="1" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="75" t="s">
+      <c r="C7" s="98" t="s">
         <v>35</v>
       </c>
       <c r="D7" s="46" t="s">
@@ -3802,7 +3808,7 @@
       <c r="E7" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="126"/>
+      <c r="F7" s="81"/>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
@@ -4026,12 +4032,12 @@
       <c r="HV7" s="12"/>
     </row>
     <row r="8" spans="1:230" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="72"/>
-      <c r="B8" s="76"/>
-      <c r="C8" s="76"/>
+      <c r="A8" s="78"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="97"/>
       <c r="D8" s="46"/>
       <c r="E8" s="48"/>
-      <c r="F8" s="117"/>
+      <c r="F8" s="82"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
@@ -4255,12 +4261,12 @@
       <c r="HV8" s="12"/>
     </row>
     <row r="9" spans="1:230" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="72"/>
-      <c r="B9" s="76"/>
-      <c r="C9" s="76"/>
+      <c r="A9" s="78"/>
+      <c r="B9" s="97"/>
+      <c r="C9" s="97"/>
       <c r="D9" s="46"/>
       <c r="E9" s="48"/>
-      <c r="F9" s="117"/>
+      <c r="F9" s="82"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
@@ -4713,13 +4719,13 @@
       <c r="HV10"/>
     </row>
     <row r="11" spans="1:230" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="71">
+      <c r="A11" s="77">
         <v>2</v>
       </c>
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="75" t="s">
+      <c r="C11" s="98" t="s">
         <v>51</v>
       </c>
       <c r="D11" s="46" t="s">
@@ -4728,7 +4734,7 @@
       <c r="E11" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="127"/>
+      <c r="F11" s="83"/>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
@@ -4952,14 +4958,14 @@
       <c r="HV11" s="12"/>
     </row>
     <row r="12" spans="1:230" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="72"/>
-      <c r="B12" s="76"/>
-      <c r="C12" s="76"/>
+      <c r="A12" s="78"/>
+      <c r="B12" s="97"/>
+      <c r="C12" s="97"/>
       <c r="D12" s="46" t="s">
         <v>82</v>
       </c>
       <c r="E12" s="47"/>
-      <c r="F12" s="118"/>
+      <c r="F12" s="84"/>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
@@ -5183,14 +5189,14 @@
       <c r="HV12" s="12"/>
     </row>
     <row r="13" spans="1:230" s="8" customFormat="1" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="72"/>
-      <c r="B13" s="76"/>
-      <c r="C13" s="76"/>
+      <c r="A13" s="78"/>
+      <c r="B13" s="97"/>
+      <c r="C13" s="97"/>
       <c r="D13" s="46" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="47"/>
-      <c r="F13" s="118"/>
+      <c r="F13" s="84"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
@@ -5643,13 +5649,13 @@
       <c r="HV14"/>
     </row>
     <row r="15" spans="1:230" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="77" t="s">
+      <c r="A15" s="128" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="80" t="s">
+      <c r="B15" s="104" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="80" t="s">
+      <c r="C15" s="104" t="s">
         <v>52</v>
       </c>
       <c r="D15" s="46" t="s">
@@ -5658,7 +5664,7 @@
       <c r="E15" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="126"/>
+      <c r="F15" s="81"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
@@ -5882,14 +5888,14 @@
       <c r="HV15" s="12"/>
     </row>
     <row r="16" spans="1:230" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="78"/>
-      <c r="B16" s="81"/>
-      <c r="C16" s="81"/>
+      <c r="A16" s="91"/>
+      <c r="B16" s="105"/>
+      <c r="C16" s="105"/>
       <c r="D16" s="46" t="s">
         <v>81</v>
       </c>
       <c r="E16" s="48"/>
-      <c r="F16" s="117"/>
+      <c r="F16" s="82"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
@@ -6113,12 +6119,12 @@
       <c r="HV16" s="12"/>
     </row>
     <row r="17" spans="1:230" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="79"/>
-      <c r="B17" s="82"/>
-      <c r="C17" s="82"/>
+      <c r="A17" s="92"/>
+      <c r="B17" s="106"/>
+      <c r="C17" s="106"/>
       <c r="D17" s="46"/>
       <c r="E17" s="48"/>
-      <c r="F17" s="117"/>
+      <c r="F17" s="82"/>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
@@ -6571,13 +6577,13 @@
       <c r="HV18"/>
     </row>
     <row r="19" spans="1:230" s="8" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="71" t="s">
+      <c r="A19" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="75" t="s">
+      <c r="B19" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="75" t="s">
+      <c r="C19" s="98" t="s">
         <v>53</v>
       </c>
       <c r="D19" s="46" t="s">
@@ -6586,7 +6592,7 @@
       <c r="E19" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="116"/>
+      <c r="F19" s="85"/>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
@@ -6810,14 +6816,14 @@
       <c r="HV19" s="12"/>
     </row>
     <row r="20" spans="1:230" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="72"/>
-      <c r="B20" s="76"/>
-      <c r="C20" s="76"/>
+      <c r="A20" s="78"/>
+      <c r="B20" s="97"/>
+      <c r="C20" s="97"/>
       <c r="D20" s="46" t="s">
         <v>83</v>
       </c>
       <c r="E20" s="48"/>
-      <c r="F20" s="117"/>
+      <c r="F20" s="82"/>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
@@ -7041,12 +7047,12 @@
       <c r="HV20" s="12"/>
     </row>
     <row r="21" spans="1:230" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="72"/>
-      <c r="B21" s="76"/>
-      <c r="C21" s="76"/>
+      <c r="A21" s="78"/>
+      <c r="B21" s="97"/>
+      <c r="C21" s="97"/>
       <c r="D21" s="46"/>
       <c r="E21" s="48"/>
-      <c r="F21" s="117"/>
+      <c r="F21" s="82"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
@@ -7499,13 +7505,13 @@
       <c r="HV22"/>
     </row>
     <row r="23" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="71">
+      <c r="A23" s="77">
         <v>5</v>
       </c>
-      <c r="B23" s="75" t="s">
+      <c r="B23" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="75" t="s">
+      <c r="C23" s="98" t="s">
         <v>37</v>
       </c>
       <c r="D23" s="46" t="s">
@@ -7514,27 +7520,27 @@
       <c r="E23" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="119"/>
+      <c r="F23" s="86"/>
     </row>
     <row r="24" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="72"/>
-      <c r="B24" s="76"/>
-      <c r="C24" s="76"/>
+      <c r="A24" s="78"/>
+      <c r="B24" s="97"/>
+      <c r="C24" s="97"/>
       <c r="D24" s="46" t="s">
         <v>39</v>
       </c>
       <c r="E24" s="48"/>
-      <c r="F24" s="120"/>
+      <c r="F24" s="73"/>
     </row>
     <row r="25" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="72"/>
-      <c r="B25" s="76"/>
-      <c r="C25" s="76"/>
+      <c r="A25" s="78"/>
+      <c r="B25" s="97"/>
+      <c r="C25" s="97"/>
       <c r="D25" s="46" t="s">
         <v>40</v>
       </c>
       <c r="E25" s="48"/>
-      <c r="F25" s="120"/>
+      <c r="F25" s="73"/>
     </row>
     <row r="26" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="37"/>
@@ -7545,13 +7551,13 @@
       <c r="F26" s="51"/>
     </row>
     <row r="27" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="71">
+      <c r="A27" s="77">
         <v>6</v>
       </c>
-      <c r="B27" s="75" t="s">
+      <c r="B27" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="75" t="s">
+      <c r="C27" s="98" t="s">
         <v>43</v>
       </c>
       <c r="D27" s="46" t="s">
@@ -7560,27 +7566,27 @@
       <c r="E27" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="119"/>
+      <c r="F27" s="86"/>
     </row>
     <row r="28" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="72"/>
-      <c r="B28" s="76"/>
-      <c r="C28" s="76"/>
+      <c r="A28" s="78"/>
+      <c r="B28" s="97"/>
+      <c r="C28" s="97"/>
       <c r="D28" s="46" t="s">
         <v>45</v>
       </c>
       <c r="E28" s="48"/>
-      <c r="F28" s="121"/>
+      <c r="F28" s="75"/>
     </row>
     <row r="29" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="72"/>
-      <c r="B29" s="76"/>
-      <c r="C29" s="76"/>
+      <c r="A29" s="78"/>
+      <c r="B29" s="97"/>
+      <c r="C29" s="97"/>
       <c r="D29" s="46" t="s">
         <v>40</v>
       </c>
       <c r="E29" s="48"/>
-      <c r="F29" s="121"/>
+      <c r="F29" s="75"/>
     </row>
     <row r="30" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="37"/>
@@ -7590,60 +7596,60 @@
       <c r="E30" s="50"/>
     </row>
     <row r="31" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="71">
+      <c r="A31" s="77">
         <v>7</v>
       </c>
-      <c r="B31" s="75" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="75" t="s">
+      <c r="B31" s="98" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="98" t="s">
         <v>47</v>
       </c>
       <c r="D31" s="46" t="s">
         <v>38</v>
       </c>
       <c r="E31" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="F31" s="119"/>
+        <v>87</v>
+      </c>
+      <c r="F31" s="86"/>
     </row>
     <row r="32" spans="1:230" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="101"/>
-      <c r="B32" s="76"/>
-      <c r="C32" s="76"/>
+      <c r="A32" s="108"/>
+      <c r="B32" s="97"/>
+      <c r="C32" s="97"/>
       <c r="D32" s="46" t="s">
         <v>45</v>
       </c>
       <c r="E32" s="48"/>
-      <c r="F32" s="121"/>
+      <c r="F32" s="75"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="101"/>
-      <c r="B33" s="76"/>
-      <c r="C33" s="76"/>
+      <c r="A33" s="108"/>
+      <c r="B33" s="97"/>
+      <c r="C33" s="97"/>
       <c r="D33" s="46" t="s">
         <v>40</v>
       </c>
       <c r="E33" s="48"/>
-      <c r="F33" s="121"/>
+      <c r="F33" s="75"/>
     </row>
     <row r="34" spans="1:6" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="102" t="s">
+      <c r="A34" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="103"/>
-      <c r="C34" s="103"/>
-      <c r="D34" s="103"/>
-      <c r="E34" s="103"/>
+      <c r="B34" s="110"/>
+      <c r="C34" s="110"/>
+      <c r="D34" s="110"/>
+      <c r="E34" s="110"/>
     </row>
     <row r="35" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="71">
+      <c r="A35" s="77">
         <v>8</v>
       </c>
-      <c r="B35" s="75" t="s">
+      <c r="B35" s="98" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="75" t="s">
+      <c r="C35" s="98" t="s">
         <v>50</v>
       </c>
       <c r="D35" s="46" t="s">
@@ -7652,31 +7658,31 @@
       <c r="E35" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="F35" s="125"/>
+      <c r="F35" s="74"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="72"/>
-      <c r="B36" s="76"/>
-      <c r="C36" s="76"/>
+      <c r="A36" s="78"/>
+      <c r="B36" s="97"/>
+      <c r="C36" s="97"/>
       <c r="D36" s="46"/>
       <c r="E36" s="48"/>
-      <c r="F36" s="121"/>
+      <c r="F36" s="75"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="72"/>
-      <c r="B37" s="76"/>
-      <c r="C37" s="76"/>
+      <c r="A37" s="78"/>
+      <c r="B37" s="97"/>
+      <c r="C37" s="97"/>
       <c r="D37" s="46"/>
       <c r="E37" s="48"/>
-      <c r="F37" s="121"/>
+      <c r="F37" s="75"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="72"/>
-      <c r="B38" s="76"/>
-      <c r="C38" s="76"/>
+      <c r="A38" s="78"/>
+      <c r="B38" s="97"/>
+      <c r="C38" s="97"/>
       <c r="D38" s="46"/>
       <c r="E38" s="48"/>
-      <c r="F38" s="121"/>
+      <c r="F38" s="75"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="37"/>
@@ -7686,13 +7692,13 @@
       <c r="E39" s="50"/>
     </row>
     <row r="40" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="71">
+      <c r="A40" s="77">
         <v>9</v>
       </c>
-      <c r="B40" s="75" t="s">
+      <c r="B40" s="98" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="99" t="s">
+      <c r="C40" s="107" t="s">
         <v>54</v>
       </c>
       <c r="D40" s="46" t="s">
@@ -7701,25 +7707,25 @@
       <c r="E40" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="F40" s="125"/>
+      <c r="F40" s="74"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="72"/>
-      <c r="B41" s="76"/>
-      <c r="C41" s="81"/>
+      <c r="A41" s="78"/>
+      <c r="B41" s="97"/>
+      <c r="C41" s="105"/>
       <c r="D41" s="46" t="s">
         <v>17</v>
       </c>
       <c r="E41" s="48"/>
-      <c r="F41" s="121"/>
+      <c r="F41" s="75"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="72"/>
-      <c r="B42" s="76"/>
-      <c r="C42" s="100"/>
+      <c r="A42" s="78"/>
+      <c r="B42" s="97"/>
+      <c r="C42" s="96"/>
       <c r="D42" s="46"/>
       <c r="E42" s="48"/>
-      <c r="F42" s="121"/>
+      <c r="F42" s="75"/>
     </row>
     <row r="43" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="37"/>
@@ -7729,13 +7735,13 @@
       <c r="E43" s="39"/>
     </row>
     <row r="44" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="71">
+      <c r="A44" s="77">
         <v>10</v>
       </c>
-      <c r="B44" s="80" t="s">
+      <c r="B44" s="104" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="99" t="s">
+      <c r="C44" s="107" t="s">
         <v>50</v>
       </c>
       <c r="D44" s="46" t="s">
@@ -7744,23 +7750,23 @@
       <c r="E44" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="F44" s="120"/>
+      <c r="F44" s="73"/>
     </row>
     <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="72"/>
-      <c r="B45" s="81"/>
-      <c r="C45" s="81"/>
+      <c r="A45" s="78"/>
+      <c r="B45" s="105"/>
+      <c r="C45" s="105"/>
       <c r="D45" s="46"/>
       <c r="E45" s="48"/>
-      <c r="F45" s="120"/>
+      <c r="F45" s="73"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="72"/>
-      <c r="B46" s="82"/>
-      <c r="C46" s="82"/>
+      <c r="A46" s="78"/>
+      <c r="B46" s="106"/>
+      <c r="C46" s="106"/>
       <c r="D46" s="52"/>
       <c r="E46" s="48"/>
-      <c r="F46" s="120"/>
+      <c r="F46" s="73"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="37"/>
@@ -7771,13 +7777,13 @@
       <c r="F47" s="51"/>
     </row>
     <row r="48" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="71">
+      <c r="A48" s="77">
         <v>11</v>
       </c>
-      <c r="B48" s="106" t="s">
+      <c r="B48" s="99" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="106" t="s">
+      <c r="C48" s="99" t="s">
         <v>64</v>
       </c>
       <c r="D48" s="46" t="s">
@@ -7786,23 +7792,23 @@
       <c r="E48" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="F48" s="120"/>
+      <c r="F48" s="73"/>
     </row>
     <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="72"/>
-      <c r="B49" s="107"/>
-      <c r="C49" s="107"/>
+      <c r="A49" s="78"/>
+      <c r="B49" s="100"/>
+      <c r="C49" s="100"/>
       <c r="D49" s="46"/>
       <c r="E49" s="48"/>
-      <c r="F49" s="120"/>
+      <c r="F49" s="73"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="72"/>
-      <c r="B50" s="108"/>
-      <c r="C50" s="108"/>
+      <c r="A50" s="78"/>
+      <c r="B50" s="101"/>
+      <c r="C50" s="101"/>
       <c r="D50" s="52"/>
       <c r="E50" s="53"/>
-      <c r="F50" s="120"/>
+      <c r="F50" s="73"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="37"/>
@@ -7813,13 +7819,13 @@
       <c r="F51" s="51"/>
     </row>
     <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A52" s="71">
+      <c r="A52" s="77">
         <v>12</v>
       </c>
-      <c r="B52" s="104" t="s">
+      <c r="B52" s="102" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="105" t="s">
+      <c r="C52" s="103" t="s">
         <v>66</v>
       </c>
       <c r="D52" s="55" t="s">
@@ -7828,44 +7834,44 @@
       <c r="E52" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="F52" s="123"/>
+      <c r="F52" s="76"/>
     </row>
     <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A53" s="72"/>
-      <c r="B53" s="104"/>
-      <c r="C53" s="105"/>
+      <c r="A53" s="78"/>
+      <c r="B53" s="102"/>
+      <c r="C53" s="103"/>
       <c r="D53" s="57"/>
       <c r="E53" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="F53" s="123"/>
+      <c r="F53" s="76"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="72"/>
-      <c r="B54" s="104"/>
-      <c r="C54" s="105"/>
+      <c r="A54" s="78"/>
+      <c r="B54" s="102"/>
+      <c r="C54" s="103"/>
       <c r="D54" s="58"/>
       <c r="E54" s="59"/>
-      <c r="F54" s="123"/>
+      <c r="F54" s="76"/>
     </row>
     <row r="55" spans="1:6" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="109" t="s">
+      <c r="A55" s="88" t="s">
         <v>67</v>
       </c>
-      <c r="B55" s="110"/>
-      <c r="C55" s="110"/>
-      <c r="D55" s="110"/>
-      <c r="E55" s="110"/>
+      <c r="B55" s="89"/>
+      <c r="C55" s="89"/>
+      <c r="D55" s="89"/>
+      <c r="E55" s="89"/>
       <c r="F55" s="51"/>
     </row>
     <row r="56" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A56" s="71">
+      <c r="A56" s="77">
         <v>13</v>
       </c>
-      <c r="B56" s="104" t="s">
+      <c r="B56" s="102" t="s">
         <v>68</v>
       </c>
-      <c r="C56" s="105" t="s">
+      <c r="C56" s="103" t="s">
         <v>69</v>
       </c>
       <c r="D56" s="55" t="s">
@@ -7874,27 +7880,27 @@
       <c r="E56" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="F56" s="122"/>
+      <c r="F56" s="71"/>
     </row>
     <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A57" s="72"/>
-      <c r="B57" s="104"/>
-      <c r="C57" s="105"/>
+      <c r="A57" s="78"/>
+      <c r="B57" s="102"/>
+      <c r="C57" s="103"/>
       <c r="D57" s="61" t="s">
         <v>71</v>
       </c>
       <c r="E57" s="62"/>
-      <c r="F57" s="122"/>
+      <c r="F57" s="71"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="72"/>
-      <c r="B58" s="104"/>
-      <c r="C58" s="105"/>
+      <c r="A58" s="78"/>
+      <c r="B58" s="102"/>
+      <c r="C58" s="103"/>
       <c r="D58" s="63" t="s">
         <v>76</v>
       </c>
       <c r="E58" s="64"/>
-      <c r="F58" s="122"/>
+      <c r="F58" s="71"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="37"/>
@@ -7905,13 +7911,13 @@
       <c r="F59" s="51"/>
     </row>
     <row r="60" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="71">
+      <c r="A60" s="77">
         <v>14</v>
       </c>
-      <c r="B60" s="104" t="s">
+      <c r="B60" s="102" t="s">
         <v>72</v>
       </c>
-      <c r="C60" s="105" t="s">
+      <c r="C60" s="103" t="s">
         <v>73</v>
       </c>
       <c r="D60" s="66" t="s">
@@ -7920,27 +7926,27 @@
       <c r="E60" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="F60" s="124"/>
+      <c r="F60" s="72"/>
     </row>
     <row r="61" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A61" s="72"/>
-      <c r="B61" s="104"/>
-      <c r="C61" s="104"/>
+      <c r="A61" s="78"/>
+      <c r="B61" s="102"/>
+      <c r="C61" s="102"/>
       <c r="D61" s="67" t="s">
         <v>71</v>
       </c>
       <c r="E61" s="67"/>
-      <c r="F61" s="124"/>
+      <c r="F61" s="72"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="72"/>
-      <c r="B62" s="104"/>
-      <c r="C62" s="104"/>
+      <c r="A62" s="78"/>
+      <c r="B62" s="102"/>
+      <c r="C62" s="102"/>
       <c r="D62" s="67" t="s">
         <v>78</v>
       </c>
       <c r="E62" s="67"/>
-      <c r="F62" s="124"/>
+      <c r="F62" s="72"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="37"/>
@@ -7951,13 +7957,13 @@
       <c r="F63" s="51"/>
     </row>
     <row r="64" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="71">
+      <c r="A64" s="77">
         <v>15</v>
       </c>
-      <c r="B64" s="100" t="s">
+      <c r="B64" s="96" t="s">
         <v>74</v>
       </c>
-      <c r="C64" s="100" t="s">
+      <c r="C64" s="96" t="s">
         <v>75</v>
       </c>
       <c r="D64" s="46" t="s">
@@ -7966,27 +7972,27 @@
       <c r="E64" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="F64" s="120"/>
+      <c r="F64" s="73"/>
     </row>
     <row r="65" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="72"/>
-      <c r="B65" s="76"/>
-      <c r="C65" s="76"/>
+      <c r="A65" s="78"/>
+      <c r="B65" s="97"/>
+      <c r="C65" s="97"/>
       <c r="D65" s="46" t="s">
         <v>71</v>
       </c>
       <c r="E65" s="48"/>
-      <c r="F65" s="120"/>
+      <c r="F65" s="73"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="72"/>
-      <c r="B66" s="76"/>
-      <c r="C66" s="76"/>
+      <c r="A66" s="78"/>
+      <c r="B66" s="97"/>
+      <c r="C66" s="97"/>
       <c r="D66" s="46" t="s">
         <v>79</v>
       </c>
       <c r="E66" s="48"/>
-      <c r="F66" s="120"/>
+      <c r="F66" s="73"/>
     </row>
     <row r="67" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="37"/>
@@ -7997,11 +8003,11 @@
       <c r="F67" s="51"/>
     </row>
     <row r="68" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="71">
+      <c r="A68" s="77">
         <v>16</v>
       </c>
-      <c r="B68" s="75"/>
-      <c r="C68" s="75" t="s">
+      <c r="B68" s="98"/>
+      <c r="C68" s="98" t="s">
         <v>17</v>
       </c>
       <c r="D68" s="46"/>
@@ -8009,17 +8015,17 @@
       <c r="F68" s="51"/>
     </row>
     <row r="69" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="72"/>
-      <c r="B69" s="76"/>
-      <c r="C69" s="76"/>
+      <c r="A69" s="78"/>
+      <c r="B69" s="97"/>
+      <c r="C69" s="97"/>
       <c r="D69" s="46"/>
       <c r="E69" s="48"/>
       <c r="F69" s="51"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="72"/>
-      <c r="B70" s="76"/>
-      <c r="C70" s="76"/>
+      <c r="A70" s="78"/>
+      <c r="B70" s="97"/>
+      <c r="C70" s="97"/>
       <c r="D70" s="46"/>
       <c r="E70" s="48"/>
       <c r="F70" s="51"/>
@@ -8034,25 +8040,25 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="71">
+      <c r="A72" s="77">
         <v>17</v>
       </c>
-      <c r="B72" s="73"/>
-      <c r="C72" s="73"/>
+      <c r="B72" s="79"/>
+      <c r="C72" s="79"/>
       <c r="D72" s="40"/>
       <c r="E72" s="41"/>
     </row>
     <row r="73" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="72"/>
-      <c r="B73" s="115"/>
-      <c r="C73" s="115"/>
+      <c r="A73" s="78"/>
+      <c r="B73" s="87"/>
+      <c r="C73" s="87"/>
       <c r="D73" s="40"/>
       <c r="E73" s="41"/>
     </row>
     <row r="74" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="72"/>
-      <c r="B74" s="115"/>
-      <c r="C74" s="115"/>
+      <c r="A74" s="78"/>
+      <c r="B74" s="87"/>
+      <c r="C74" s="87"/>
       <c r="D74" s="42" t="s">
         <v>16</v>
       </c>
@@ -8068,25 +8074,25 @@
       <c r="E75" s="39"/>
     </row>
     <row r="76" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="71">
+      <c r="A76" s="77">
         <v>18</v>
       </c>
-      <c r="B76" s="73"/>
-      <c r="C76" s="73"/>
+      <c r="B76" s="79"/>
+      <c r="C76" s="79"/>
       <c r="D76" s="40"/>
       <c r="E76" s="41"/>
     </row>
     <row r="77" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="72"/>
-      <c r="B77" s="115"/>
-      <c r="C77" s="115"/>
+      <c r="A77" s="78"/>
+      <c r="B77" s="87"/>
+      <c r="C77" s="87"/>
       <c r="D77" s="40"/>
       <c r="E77" s="41"/>
     </row>
     <row r="78" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="72"/>
-      <c r="B78" s="115"/>
-      <c r="C78" s="115"/>
+      <c r="A78" s="78"/>
+      <c r="B78" s="87"/>
+      <c r="C78" s="87"/>
       <c r="D78" s="42" t="s">
         <v>16</v>
       </c>
@@ -8102,23 +8108,23 @@
       <c r="E79" s="39"/>
     </row>
     <row r="80" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="71"/>
-      <c r="B80" s="73"/>
-      <c r="C80" s="73"/>
+      <c r="A80" s="77"/>
+      <c r="B80" s="79"/>
+      <c r="C80" s="79"/>
       <c r="D80" s="40"/>
       <c r="E80" s="41"/>
     </row>
     <row r="81" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="72"/>
-      <c r="B81" s="74"/>
-      <c r="C81" s="74"/>
+      <c r="A81" s="78"/>
+      <c r="B81" s="80"/>
+      <c r="C81" s="80"/>
       <c r="D81" s="40"/>
       <c r="E81" s="41"/>
     </row>
     <row r="82" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="72"/>
-      <c r="B82" s="74"/>
-      <c r="C82" s="74"/>
+      <c r="A82" s="78"/>
+      <c r="B82" s="80"/>
+      <c r="C82" s="80"/>
       <c r="D82" s="40"/>
       <c r="E82" s="41"/>
     </row>
@@ -8130,23 +8136,23 @@
       <c r="E83" s="44"/>
     </row>
     <row r="84" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="71"/>
-      <c r="B84" s="73"/>
-      <c r="C84" s="73"/>
+      <c r="A84" s="77"/>
+      <c r="B84" s="79"/>
+      <c r="C84" s="79"/>
       <c r="D84" s="40"/>
       <c r="E84" s="41"/>
     </row>
     <row r="85" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="72"/>
-      <c r="B85" s="74"/>
-      <c r="C85" s="74"/>
+      <c r="A85" s="78"/>
+      <c r="B85" s="80"/>
+      <c r="C85" s="80"/>
       <c r="D85" s="40"/>
       <c r="E85" s="41"/>
     </row>
     <row r="86" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="72"/>
-      <c r="B86" s="74"/>
-      <c r="C86" s="74"/>
+      <c r="A86" s="78"/>
+      <c r="B86" s="80"/>
+      <c r="C86" s="80"/>
       <c r="D86" s="40"/>
       <c r="E86" s="41"/>
     </row>
@@ -8158,23 +8164,23 @@
       <c r="E87" s="44"/>
     </row>
     <row r="88" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="71"/>
-      <c r="B88" s="73"/>
-      <c r="C88" s="73"/>
+      <c r="A88" s="77"/>
+      <c r="B88" s="79"/>
+      <c r="C88" s="79"/>
       <c r="D88" s="40"/>
       <c r="E88" s="41"/>
     </row>
     <row r="89" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="72"/>
-      <c r="B89" s="74"/>
-      <c r="C89" s="74"/>
+      <c r="A89" s="78"/>
+      <c r="B89" s="80"/>
+      <c r="C89" s="80"/>
       <c r="D89" s="40"/>
       <c r="E89" s="41"/>
     </row>
     <row r="90" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="72"/>
-      <c r="B90" s="74"/>
-      <c r="C90" s="74"/>
+      <c r="A90" s="78"/>
+      <c r="B90" s="80"/>
+      <c r="C90" s="80"/>
       <c r="D90" s="40"/>
       <c r="E90" s="41"/>
     </row>
@@ -8186,23 +8192,23 @@
       <c r="E91" s="44"/>
     </row>
     <row r="92" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="71"/>
-      <c r="B92" s="73"/>
-      <c r="C92" s="73"/>
+      <c r="A92" s="77"/>
+      <c r="B92" s="79"/>
+      <c r="C92" s="79"/>
       <c r="D92" s="40"/>
       <c r="E92" s="41"/>
     </row>
     <row r="93" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="72"/>
-      <c r="B93" s="74"/>
-      <c r="C93" s="74"/>
+      <c r="A93" s="78"/>
+      <c r="B93" s="80"/>
+      <c r="C93" s="80"/>
       <c r="D93" s="40"/>
       <c r="E93" s="41"/>
     </row>
     <row r="94" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="72"/>
-      <c r="B94" s="74"/>
-      <c r="C94" s="74"/>
+      <c r="A94" s="78"/>
+      <c r="B94" s="80"/>
+      <c r="C94" s="80"/>
       <c r="D94" s="40"/>
       <c r="E94" s="41"/>
     </row>
@@ -8214,23 +8220,23 @@
       <c r="E95" s="44"/>
     </row>
     <row r="96" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="71"/>
-      <c r="B96" s="73"/>
-      <c r="C96" s="73"/>
+      <c r="A96" s="77"/>
+      <c r="B96" s="79"/>
+      <c r="C96" s="79"/>
       <c r="D96" s="40"/>
       <c r="E96" s="41"/>
     </row>
     <row r="97" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="72"/>
-      <c r="B97" s="74"/>
-      <c r="C97" s="74"/>
+      <c r="A97" s="78"/>
+      <c r="B97" s="80"/>
+      <c r="C97" s="80"/>
       <c r="D97" s="40"/>
       <c r="E97" s="41"/>
     </row>
     <row r="98" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="72"/>
-      <c r="B98" s="74"/>
-      <c r="C98" s="74"/>
+      <c r="A98" s="78"/>
+      <c r="B98" s="80"/>
+      <c r="C98" s="80"/>
       <c r="D98" s="40"/>
       <c r="E98" s="41"/>
     </row>
@@ -8242,23 +8248,23 @@
       <c r="E99" s="44"/>
     </row>
     <row r="100" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="71"/>
-      <c r="B100" s="73"/>
-      <c r="C100" s="73"/>
+      <c r="A100" s="77"/>
+      <c r="B100" s="79"/>
+      <c r="C100" s="79"/>
       <c r="D100" s="40"/>
       <c r="E100" s="41"/>
     </row>
     <row r="101" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="72"/>
-      <c r="B101" s="74"/>
-      <c r="C101" s="74"/>
+      <c r="A101" s="78"/>
+      <c r="B101" s="80"/>
+      <c r="C101" s="80"/>
       <c r="D101" s="40"/>
       <c r="E101" s="41"/>
     </row>
     <row r="102" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="72"/>
-      <c r="B102" s="74"/>
-      <c r="C102" s="74"/>
+      <c r="A102" s="78"/>
+      <c r="B102" s="80"/>
+      <c r="C102" s="80"/>
       <c r="D102" s="40"/>
       <c r="E102" s="41"/>
     </row>
@@ -8270,23 +8276,23 @@
       <c r="E103" s="44"/>
     </row>
     <row r="104" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="71"/>
-      <c r="B104" s="73"/>
-      <c r="C104" s="73"/>
+      <c r="A104" s="77"/>
+      <c r="B104" s="79"/>
+      <c r="C104" s="79"/>
       <c r="D104" s="40"/>
       <c r="E104" s="41"/>
     </row>
     <row r="105" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="72"/>
-      <c r="B105" s="74"/>
-      <c r="C105" s="74"/>
+      <c r="A105" s="78"/>
+      <c r="B105" s="80"/>
+      <c r="C105" s="80"/>
       <c r="D105" s="40"/>
       <c r="E105" s="41"/>
     </row>
     <row r="106" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="72"/>
-      <c r="B106" s="74"/>
-      <c r="C106" s="74"/>
+      <c r="A106" s="78"/>
+      <c r="B106" s="80"/>
+      <c r="C106" s="80"/>
       <c r="D106" s="40"/>
       <c r="E106" s="41"/>
     </row>
@@ -8298,23 +8304,23 @@
       <c r="E107" s="44"/>
     </row>
     <row r="108" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="71"/>
-      <c r="B108" s="73"/>
-      <c r="C108" s="73"/>
+      <c r="A108" s="77"/>
+      <c r="B108" s="79"/>
+      <c r="C108" s="79"/>
       <c r="D108" s="40"/>
       <c r="E108" s="41"/>
     </row>
     <row r="109" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="72"/>
-      <c r="B109" s="74"/>
-      <c r="C109" s="74"/>
+      <c r="A109" s="78"/>
+      <c r="B109" s="80"/>
+      <c r="C109" s="80"/>
       <c r="D109" s="40"/>
       <c r="E109" s="41"/>
     </row>
     <row r="110" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="72"/>
-      <c r="B110" s="74"/>
-      <c r="C110" s="74"/>
+      <c r="A110" s="78"/>
+      <c r="B110" s="80"/>
+      <c r="C110" s="80"/>
       <c r="D110" s="40"/>
       <c r="E110" s="41"/>
     </row>
@@ -8326,23 +8332,23 @@
       <c r="E111" s="44"/>
     </row>
     <row r="112" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="71"/>
-      <c r="B112" s="73"/>
-      <c r="C112" s="73"/>
+      <c r="A112" s="77"/>
+      <c r="B112" s="79"/>
+      <c r="C112" s="79"/>
       <c r="D112" s="40"/>
       <c r="E112" s="41"/>
     </row>
     <row r="113" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="72"/>
-      <c r="B113" s="74"/>
-      <c r="C113" s="74"/>
+      <c r="A113" s="78"/>
+      <c r="B113" s="80"/>
+      <c r="C113" s="80"/>
       <c r="D113" s="40"/>
       <c r="E113" s="41"/>
     </row>
     <row r="114" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="72"/>
-      <c r="B114" s="74"/>
-      <c r="C114" s="74"/>
+      <c r="A114" s="78"/>
+      <c r="B114" s="80"/>
+      <c r="C114" s="80"/>
       <c r="D114" s="40"/>
       <c r="E114" s="41"/>
     </row>
@@ -8354,53 +8360,68 @@
       <c r="E115" s="44"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A116" s="111"/>
-      <c r="B116" s="112"/>
-      <c r="C116" s="112"/>
+      <c r="A116" s="90"/>
+      <c r="B116" s="93"/>
+      <c r="C116" s="93"/>
       <c r="D116" s="40"/>
       <c r="E116" s="41"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A117" s="78"/>
-      <c r="B117" s="113"/>
-      <c r="C117" s="113"/>
+      <c r="A117" s="91"/>
+      <c r="B117" s="94"/>
+      <c r="C117" s="94"/>
       <c r="D117" s="40"/>
       <c r="E117" s="41"/>
     </row>
     <row r="118" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="79"/>
-      <c r="B118" s="114"/>
-      <c r="C118" s="114"/>
+      <c r="A118" s="92"/>
+      <c r="B118" s="95"/>
+      <c r="C118" s="95"/>
       <c r="D118" s="40"/>
       <c r="E118" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="F60:F62"/>
-    <mergeCell ref="F64:F66"/>
-    <mergeCell ref="F35:F38"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="F48:F50"/>
-    <mergeCell ref="F52:F54"/>
-    <mergeCell ref="A88:A90"/>
-    <mergeCell ref="B88:B90"/>
-    <mergeCell ref="C88:C90"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="A76:A78"/>
-    <mergeCell ref="B76:B78"/>
-    <mergeCell ref="C76:C78"/>
-    <mergeCell ref="A80:A82"/>
-    <mergeCell ref="B80:B82"/>
-    <mergeCell ref="C80:C82"/>
-    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="A112:A114"/>
+    <mergeCell ref="B112:B114"/>
+    <mergeCell ref="C112:C114"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="B104:B106"/>
+    <mergeCell ref="C104:C106"/>
+    <mergeCell ref="A108:A110"/>
+    <mergeCell ref="B108:B110"/>
+    <mergeCell ref="C108:C110"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="E1:E4"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D4"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
     <mergeCell ref="A116:A118"/>
     <mergeCell ref="B116:B118"/>
     <mergeCell ref="C116:C118"/>
@@ -8416,6 +8437,26 @@
     <mergeCell ref="A84:A86"/>
     <mergeCell ref="B84:B86"/>
     <mergeCell ref="C84:C86"/>
+    <mergeCell ref="A100:A102"/>
+    <mergeCell ref="B100:B102"/>
+    <mergeCell ref="C100:C102"/>
+    <mergeCell ref="A92:A94"/>
+    <mergeCell ref="B92:B94"/>
+    <mergeCell ref="C92:C94"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="B96:B98"/>
+    <mergeCell ref="C96:C98"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="F31:F33"/>
+    <mergeCell ref="A76:A78"/>
+    <mergeCell ref="B76:B78"/>
+    <mergeCell ref="C76:C78"/>
+    <mergeCell ref="A55:E55"/>
     <mergeCell ref="A48:A50"/>
     <mergeCell ref="B48:B50"/>
     <mergeCell ref="C48:C50"/>
@@ -8429,60 +8470,25 @@
     <mergeCell ref="B60:B62"/>
     <mergeCell ref="C60:C62"/>
     <mergeCell ref="A44:A46"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="F60:F62"/>
+    <mergeCell ref="F64:F66"/>
+    <mergeCell ref="F35:F38"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="F48:F50"/>
+    <mergeCell ref="F52:F54"/>
+    <mergeCell ref="A88:A90"/>
+    <mergeCell ref="B88:B90"/>
+    <mergeCell ref="C88:C90"/>
+    <mergeCell ref="A80:A82"/>
+    <mergeCell ref="B80:B82"/>
+    <mergeCell ref="C80:C82"/>
     <mergeCell ref="B44:B46"/>
     <mergeCell ref="C44:C46"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
     <mergeCell ref="A40:A42"/>
     <mergeCell ref="B40:B42"/>
     <mergeCell ref="C40:C42"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="E1:E4"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A100:A102"/>
-    <mergeCell ref="B100:B102"/>
-    <mergeCell ref="C100:C102"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A92:A94"/>
-    <mergeCell ref="B92:B94"/>
-    <mergeCell ref="C92:C94"/>
-    <mergeCell ref="A96:A98"/>
-    <mergeCell ref="B96:B98"/>
-    <mergeCell ref="C96:C98"/>
-    <mergeCell ref="A112:A114"/>
-    <mergeCell ref="B112:B114"/>
-    <mergeCell ref="C112:C114"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="B104:B106"/>
-    <mergeCell ref="C104:C106"/>
-    <mergeCell ref="A108:A110"/>
-    <mergeCell ref="B108:B110"/>
-    <mergeCell ref="C108:C110"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.39370078740157483" bottom="0.39370078740157483" header="0.27559055118110237" footer="0.39370078740157483"/>

</xml_diff>